<commit_message>
v1.1-beta1.1.2.8 fix: - 修复setUp和用例page共同调用basepage的构造方法造成的bug - 调试修改unitInformationModification_page用例的问题 - 更新chromedriver驱动 - 修改basepage和basepage接口
</commit_message>
<xml_diff>
--- a/data/testdata/unitInformationModification.xlsx
+++ b/data/testdata/unitInformationModification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PublicInstitutionSystem\data\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7FB6C4-39CB-4E62-A643-6781929701ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3871A4F4-7C1B-404D-90FE-6DBE7AAEBDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="单位基础信息修改" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>统一社会信用代码</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -39,10 +39,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>测试单位三</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>单位负责人</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -74,38 +70,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>测试单位二</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>张三</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>李四</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>王五</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>部分人员</t>
-  </si>
-  <si>
-    <t>全部人员</t>
-  </si>
-  <si>
     <t>01101</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>01102</t>
-  </si>
-  <si>
-    <t>01103</t>
-  </si>
-  <si>
     <t>单位性质</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -148,30 +120,15 @@
     <t>正地厅级</t>
   </si>
   <si>
-    <t>未定级别</t>
-  </si>
-  <si>
-    <t>副地厅级</t>
-  </si>
-  <si>
     <t>否</t>
   </si>
   <si>
-    <t>是</t>
-  </si>
-  <si>
     <t>2级审核（基层-终审）</t>
   </si>
   <si>
     <t>无</t>
   </si>
   <si>
-    <t>一类区</t>
-  </si>
-  <si>
-    <t>四类区</t>
-  </si>
-  <si>
     <t>上海市</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -182,28 +139,10 @@
     <t>2864290869</t>
   </si>
   <si>
-    <t>2202499692</t>
-  </si>
-  <si>
-    <t>国家机关</t>
-  </si>
-  <si>
-    <t>机关工资制度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>15101152133</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>15131080133</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>13178922133</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>隶属关系</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -239,27 +178,15 @@
     <t>中央在京单位</t>
   </si>
   <si>
-    <t>省辖市、自治州、行署</t>
-  </si>
-  <si>
     <t>3499米以下地区</t>
   </si>
   <si>
     <t>4500米以上地区</t>
   </si>
   <si>
-    <t>3500-4499米地区</t>
-  </si>
-  <si>
     <t>生产经营类事业单位</t>
   </si>
   <si>
-    <t>公益二类事业单位</t>
-  </si>
-  <si>
-    <t>公益一类事业单位</t>
-  </si>
-  <si>
     <t>普通高等教育</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -267,13 +194,8 @@
     <t>核定收支、定额补助</t>
   </si>
   <si>
-    <t>核定收支、定项补助</t>
-  </si>
-  <si>
-    <t>核定收支、经费自筹</t>
-  </si>
-  <si>
-    <t>省、自治区、直辖市</t>
+    <t>12510501MB1Q951567</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -608,41 +530,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD4"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.44140625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5" style="1" customWidth="1"/>
+    <col min="26" max="26" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -650,73 +572,73 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
@@ -724,247 +646,123 @@
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="W2" s="1" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{92D822B2-3044-4793-B84A-72C5C0D6243F}">
+  <dataValidations count="15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{0B4E8B39-2B91-47A8-94B5-ED0D6D58D7EB}">
       <formula1>"全部人员,部分人员,无财政供养人员"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{60873097-2830-4C33-B508-C08683804433}">
-      <formula1>LEN(TRIM(A2:A287))&gt;0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{80888037-D123-4868-902A-EE6434AB1241}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{55F8F954-9E71-40DC-9547-BE321D43F7E4}">
+      <formula1>LEN(TRIM(A2:A285))&gt;0</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1048573:A1048576" xr:uid="{31AD1A47-5D47-44B3-954B-3F71F8F41B4B}">
+      <formula1>LEN(TRIM(A282:A1048573))&gt;0</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1048290:A1048572" xr:uid="{1C9144AE-D80A-4F68-BF5C-90CED7837EB4}">
+      <formula1>LEN(TRIM(A1:A1048290))&gt;0</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A1048289" xr:uid="{2BF15D39-E16F-481D-A98D-5A80CB0907C7}">
+      <formula1>LEN(TRIM(A3:A288))&gt;0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{76781BBA-D06D-495E-BEAD-1163103DF5F4}">
       <formula1>"国家机关,事业单位,参公单位,机关服务中心"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{A2F8388C-A25F-4912-8498-4D2D438CF308}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{EE914555-8F56-4123-9607-CC63B9366AC1}">
       <formula1>"正地厅级,副地厅级,正县处级,副县处级,正区科级副区科级,副科级以下,未定级别"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576 X2:X1048576" xr:uid="{1EC0A3DA-1BA4-47C3-9C95-205A7344CD89}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X1048576 M2:M1048576" xr:uid="{28D750D7-AC05-47A9-A459-C47485A4E087}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{1B0AC280-BD01-44B6-93C3-155A401BD4D9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{3FB87C6C-3BA5-436B-9E3B-9456B8E9C4C6}">
       <formula1>"3级审核（基层-主管-终审）,2级审核（基层-终审）"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048576" xr:uid="{811C3E19-A813-48E0-A1A4-520FC8225235}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048576" xr:uid="{0549B1B6-A3D1-4303-B85E-C4410DB04571}">
       <formula1>"一类区,二类区,三类区,四类区,五类区,六类区,无"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{2AD87058-07F0-4EC7-9499-80C857F9FDA8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{B762CD24-B94E-4962-95AC-3AF431AA919C}">
       <formula1>"全部人员,部分人员,无财政统发人员"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R1048576" xr:uid="{CA46AB37-F759-42DD-ADB3-602DDD17A2CA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R1048576" xr:uid="{482E54D2-E021-49E2-91F2-5ACD92F8E1D4}">
       <formula1>"中央,中央在京单位,省、自治区、直辖市,省辖市、自治州、行署,县、市、区,乡、镇"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:U1048576" xr:uid="{60248A7B-F438-4A6B-B211-D3E0CCA8C68F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:U1048576" xr:uid="{80FD85EC-C390-4673-A256-45CAE33E4719}">
       <formula1>"3499米以下地区,3500-4499米地区,4500米以上地区"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576" xr:uid="{22CAA0DB-4EE8-4296-83F5-640A5027169A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576" xr:uid="{18AE59E7-4E14-4C46-95DF-A9FBEA7D9774}">
       <formula1>"公益一类事业单位,公益二类事业单位,生产经营类事业单位,尚未分类单位"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2:Y1048576" xr:uid="{6E1AC129-55DE-4FC6-873F-793605FCD476}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2:Y1048576" xr:uid="{4D55DF16-466D-4DC1-8D57-5CAD95C144B8}">
       <formula1>"核定收支、定额补助,核定收支、定项补助,核定收支、经费自筹"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v1.5.09 other: Fix some issues.
</commit_message>
<xml_diff>
--- a/data/testdata/unitInformationModification.xlsx
+++ b/data/testdata/unitInformationModification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PublicInstitutionSystem\data\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F71DC6-64AA-4197-9667-481A7257BB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38669480-AC8F-4334-A66D-238EF018278E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6165" yWindow="3360" windowWidth="21165" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitInformationModification" sheetId="1" r:id="rId1"/>
@@ -23,11 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="161">
-  <si>
-    <t>统一社会信用代码</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="159">
   <si>
     <t>单位名称</t>
     <phoneticPr fontId="19" type="noConversion"/>
@@ -545,11 +541,8 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>11510322MB1972530K</t>
+    <t>测试主管单位</t>
     <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>中国共产党盐边县委员会办公室</t>
   </si>
 </sst>
 </file>
@@ -2046,41 +2039,40 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.625" style="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="34" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.125" style="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" style="34" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" style="33"/>
-    <col min="11" max="11" width="17.25" style="33" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" style="33"/>
-    <col min="13" max="13" width="13" style="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" style="33"/>
-    <col min="15" max="15" width="21.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9" style="33"/>
-    <col min="17" max="17" width="29.625" style="33" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11" style="33" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9" style="33"/>
-    <col min="20" max="20" width="15.375" style="33" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.75" style="33" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.25" style="33" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="13" style="33" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.25" style="33" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9" style="33"/>
+    <col min="1" max="1" width="13" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.125" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="33"/>
+    <col min="10" max="10" width="17.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="33"/>
+    <col min="12" max="12" width="13" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="33"/>
+    <col min="14" max="14" width="21.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="33"/>
+    <col min="16" max="16" width="29.625" style="33" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" style="33" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="33"/>
+    <col min="19" max="19" width="15.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.75" style="33" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="13" style="33" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.25" style="33" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -2153,95 +2145,89 @@
       <c r="X1" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="32" t="s">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A2" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2" s="33" t="s">
+      <c r="C2" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="M2" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="M2" s="33" t="s">
-        <v>151</v>
-      </c>
       <c r="N2" s="33" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="O2" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="P2" s="33" t="str">
+        <f>IF(J2:J119="事业单位工资制度","","四川省")</f>
+        <v/>
+      </c>
+      <c r="Q2" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="R2" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="P2" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q2" s="33" t="str">
-        <f>IF(K2:K119="事业单位工资制度","","四川省")</f>
-        <v/>
-      </c>
-      <c r="R2" s="33" t="s">
-        <v>78</v>
-      </c>
       <c r="S2" s="33" t="s">
-        <v>155</v>
+        <v>86</v>
       </c>
       <c r="T2" s="33" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="U2" s="33" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="V2" s="33" t="s">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="W2" s="33" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="X2" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"是,否"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2253,85 +2239,85 @@
           <x14:formula1>
             <xm:f>'财政供养&amp;财政统发'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2</xm:sqref>
+          <xm:sqref>F2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>'财政供养&amp;财政统发'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G1048576 G1</xm:sqref>
+          <xm:sqref>F3:F1048576 F1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>'财政供养&amp;财政统发'!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>单位数据指标!$B$47:$B$50</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000006000000}">
           <x14:formula1>
             <xm:f>单位数据指标!$B$24:$B$26</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
           <x14:formula1>
             <xm:f>单位数据指标!$B$39:$B$46</xm:f>
           </x14:formula1>
-          <xm:sqref>L2</xm:sqref>
+          <xm:sqref>K2</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
             <xm:f>单位数据指标!$B$9:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>O2:O1048576</xm:sqref>
+          <xm:sqref>N2:N1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000009000000}">
           <x14:formula1>
             <xm:f>单位数据指标!$B$27:$B$33</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P1048576</xm:sqref>
+          <xm:sqref>O2:O1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000A000000}">
           <x14:formula1>
             <xm:f>单位数据指标!$B$12:$B$17</xm:f>
           </x14:formula1>
-          <xm:sqref>R2:R1048576</xm:sqref>
+          <xm:sqref>Q2:Q1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000B000000}">
           <x14:formula1>
             <xm:f>单位数据指标!$B$21:$B$23</xm:f>
           </x14:formula1>
-          <xm:sqref>T2:T1048576</xm:sqref>
+          <xm:sqref>S2:S1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000C000000}">
           <x14:formula1>
             <xm:f>单位数据指标!$B$18:$B$20</xm:f>
           </x14:formula1>
-          <xm:sqref>U2:U1048576</xm:sqref>
+          <xm:sqref>T2:T1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000D000000}">
           <x14:formula1>
             <xm:f>单位数据指标!$B$34:$B$37</xm:f>
           </x14:formula1>
-          <xm:sqref>V2:V1048576</xm:sqref>
+          <xm:sqref>U2:U1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000E000000}">
           <x14:formula1>
             <xm:f>单位数据指标!$D$3:$D$57</xm:f>
           </x14:formula1>
-          <xm:sqref>W2:W1048576</xm:sqref>
+          <xm:sqref>V2:V1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-00000F000000}">
           <x14:formula1>
             <xm:f>单位数据指标!$G$3:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Y2:Y1048576</xm:sqref>
+          <xm:sqref>X2:X1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2352,27 +2338,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2402,7 +2388,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
@@ -2413,16 +2399,16 @@
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2430,80 +2416,80 @@
     </row>
     <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="52" t="s">
+      <c r="D3" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="40"/>
       <c r="B4" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="53"/>
       <c r="D4" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="37"/>
       <c r="G4" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="41"/>
       <c r="B5" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="53"/>
       <c r="D5" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="37"/>
       <c r="G5" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="38"/>
       <c r="G6" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="40"/>
       <c r="B7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="53"/>
       <c r="D7" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2512,11 +2498,11 @@
     <row r="8" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="41"/>
       <c r="B8" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="53"/>
       <c r="D8" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2524,14 +2510,14 @@
     </row>
     <row r="9" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>152</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>153</v>
       </c>
       <c r="C9" s="53"/>
       <c r="D9" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -2540,11 +2526,11 @@
     <row r="10" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="48"/>
       <c r="B10" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10" s="53"/>
       <c r="D10" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2555,7 +2541,7 @@
       <c r="B11" s="15"/>
       <c r="C11" s="53"/>
       <c r="D11" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -2563,14 +2549,14 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="C12" s="53"/>
       <c r="D12" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -2579,11 +2565,11 @@
     <row r="13" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="40"/>
       <c r="B13" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="53"/>
       <c r="D13" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2592,11 +2578,11 @@
     <row r="14" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="40"/>
       <c r="B14" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="53"/>
       <c r="D14" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2605,11 +2591,11 @@
     <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="40"/>
       <c r="B15" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="53"/>
       <c r="D15" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -2618,11 +2604,11 @@
     <row r="16" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="40"/>
       <c r="B16" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="53"/>
       <c r="D16" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -2631,11 +2617,11 @@
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="41"/>
       <c r="B17" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="53"/>
       <c r="D17" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -2643,14 +2629,14 @@
     </row>
     <row r="18" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="C18" s="53"/>
       <c r="D18" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -2659,11 +2645,11 @@
     <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="40"/>
       <c r="B19" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" s="53"/>
       <c r="D19" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2672,11 +2658,11 @@
     <row r="20" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="41"/>
       <c r="B20" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="53"/>
       <c r="D20" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -2684,14 +2670,14 @@
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" s="39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" s="53"/>
       <c r="D21" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -2700,11 +2686,11 @@
     <row r="22" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="40"/>
       <c r="B22" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="53"/>
       <c r="D22" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -2713,11 +2699,11 @@
     <row r="23" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="41"/>
       <c r="B23" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" s="53"/>
       <c r="D23" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2725,14 +2711,14 @@
     </row>
     <row r="24" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="C24" s="53"/>
       <c r="D24" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2741,11 +2727,11 @@
     <row r="25" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" s="40"/>
       <c r="B25" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="53"/>
       <c r="D25" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -2754,11 +2740,11 @@
     <row r="26" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="41"/>
       <c r="B26" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" s="53"/>
       <c r="D26" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -2766,14 +2752,14 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="C27" s="53"/>
       <c r="D27" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -2782,11 +2768,11 @@
     <row r="28" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A28" s="40"/>
       <c r="B28" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C28" s="53"/>
       <c r="D28" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -2795,11 +2781,11 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="40"/>
       <c r="B29" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C29" s="53"/>
       <c r="D29" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2808,11 +2794,11 @@
     <row r="30" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" s="40"/>
       <c r="B30" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C30" s="53"/>
       <c r="D30" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -2821,11 +2807,11 @@
     <row r="31" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" s="40"/>
       <c r="B31" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C31" s="53"/>
       <c r="D31" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2834,11 +2820,11 @@
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40"/>
       <c r="B32" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C32" s="54"/>
       <c r="D32" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2847,11 +2833,11 @@
     <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="41"/>
       <c r="B33" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2859,14 +2845,14 @@
     </row>
     <row r="34" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2875,11 +2861,11 @@
     <row r="35" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="40"/>
       <c r="B35" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2888,11 +2874,11 @@
     <row r="36" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A36" s="40"/>
       <c r="B36" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C36" s="19"/>
       <c r="D36" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2901,11 +2887,11 @@
     <row r="37" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="40"/>
       <c r="B37" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2916,7 +2902,7 @@
       <c r="B38" s="12"/>
       <c r="C38" s="19"/>
       <c r="D38" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2924,14 +2910,14 @@
     </row>
     <row r="39" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A39" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>124</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2940,11 +2926,11 @@
     <row r="40" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="43"/>
       <c r="B40" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C40" s="19"/>
       <c r="D40" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2953,11 +2939,11 @@
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="43"/>
       <c r="B41" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2966,11 +2952,11 @@
     <row r="42" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42" s="43"/>
       <c r="B42" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C42" s="19"/>
       <c r="D42" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2979,11 +2965,11 @@
     <row r="43" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43" s="43"/>
       <c r="B43" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2992,11 +2978,11 @@
     <row r="44" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="43"/>
       <c r="B44" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C44" s="19"/>
       <c r="D44" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -3005,11 +2991,11 @@
     <row r="45" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="43"/>
       <c r="B45" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C45" s="19"/>
       <c r="D45" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -3018,11 +3004,11 @@
     <row r="46" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="43"/>
       <c r="B46" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C46" s="19"/>
       <c r="D46" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -3030,14 +3016,14 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C47" s="21"/>
       <c r="D47" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -3046,11 +3032,11 @@
     <row r="48" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="45"/>
       <c r="B48" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -3059,11 +3045,11 @@
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="45"/>
       <c r="B49" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -3072,11 +3058,11 @@
     <row r="50" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A50" s="46"/>
       <c r="B50" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -3087,7 +3073,7 @@
       <c r="B51" s="25"/>
       <c r="C51" s="26"/>
       <c r="D51" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -3098,7 +3084,7 @@
       <c r="B52" s="27"/>
       <c r="C52" s="28"/>
       <c r="D52" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -3109,7 +3095,7 @@
       <c r="B53" s="29"/>
       <c r="C53" s="30"/>
       <c r="D53" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -3120,7 +3106,7 @@
       <c r="B54" s="25"/>
       <c r="C54" s="26"/>
       <c r="D54" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -3131,7 +3117,7 @@
       <c r="B55" s="25"/>
       <c r="C55" s="26"/>
       <c r="D55" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -3142,7 +3128,7 @@
       <c r="B56" s="25"/>
       <c r="C56" s="26"/>
       <c r="D56" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -3153,7 +3139,7 @@
       <c r="B57" s="25"/>
       <c r="C57" s="26"/>
       <c r="D57" s="31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3197,34 +3183,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>